<commit_message>
Update slide switch and added links
</commit_message>
<xml_diff>
--- a/hw/ICEBoard Bill of Materials.xlsx
+++ b/hw/ICEBoard Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICEBoard\hw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgoeders\iceBoard\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B4BFCD-FA09-4C4D-89E6-D4C4157736F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09A4438-044A-4DEB-98C8-1C03D910C4B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{71482D72-135C-40BB-96C7-234F6F45C228}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{71482D72-135C-40BB-96C7-234F6F45C228}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
   <si>
     <t>Type</t>
   </si>
@@ -280,6 +286,66 @@
   </si>
   <si>
     <t>1276-6456-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/181</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1655</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=401-2002-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=CKN10889CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=TSOP38240-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=BH9V-PC-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=TC33X-103ECT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=311-100HRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=399-1099-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1276-6456-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=2104-TP124005-2CT-ND</t>
+  </si>
+  <si>
+    <t>SPDT</t>
+  </si>
+  <si>
+    <t>APEM</t>
+  </si>
+  <si>
+    <t>MHSS1104</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>679-1848-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=679-1848-ND</t>
   </si>
 </sst>
 </file>
@@ -289,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +372,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,11 +419,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -340,9 +432,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -655,27 +753,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57995C7-ECEF-42DD-8215-B17780662546}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,8 +804,11 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -727,14 +828,17 @@
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I13" si="0">G2*H2</f>
+        <f t="shared" ref="I2:I14" si="0">G2*H2</f>
         <v>22</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -760,8 +864,11 @@
       <c r="J3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -787,339 +894,423 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="K4" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="9">
         <v>0.48</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1">
-        <v>0.26</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>1.3</v>
+        <v>2.75</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1">
-        <v>1.1200000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1">
         <v>1.1200000000000001</v>
-      </c>
-      <c r="J7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1.95</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1">
         <v>1.95</v>
-      </c>
-      <c r="J8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.28000000000000003</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>1.95</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
         <v>100</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G11" s="5">
         <v>0.1</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H11" s="4">
         <v>4</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I11" s="6">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="K11" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G12" s="5">
         <v>0.1</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I12" s="6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="K12" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="5">
         <v>0.1</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H13" s="4">
         <v>8</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I13" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="K13" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>80</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G14" s="5">
         <v>0.12</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H14" s="4">
         <v>1</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="K14" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G15" s="5">
         <v>0.85</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H15" s="4">
         <v>1</v>
       </c>
-      <c r="I14" s="6">
-        <f t="shared" ref="I14" si="1">G14*H14</f>
+      <c r="I15" s="6">
+        <f t="shared" ref="I15" si="1">G15*H15</f>
         <v>0.85</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="K15" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{5D1BD6F9-23F5-4C9A-8A5F-A4F5492692CF}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{2D9D999F-B693-4FAC-8829-328C6CDB84BE}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{E2646A8C-C5E3-4FA6-A0D2-1CD01D4667FC}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{F0A7CE9B-0961-4092-B4EE-EBB031DFB683}"/>
+    <hyperlink ref="K8" r:id="rId5" xr:uid="{033F4660-D974-4D51-A875-392CE71D968A}"/>
+    <hyperlink ref="K9" r:id="rId6" xr:uid="{713BE0E6-45E9-44BE-A543-6D965D6E39A9}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{F2E7F544-9480-4746-982F-C147FD8DC0EE}"/>
+    <hyperlink ref="K11" r:id="rId8" xr:uid="{B08B6EA8-531D-4E9D-B0A0-B8B4795AEF79}"/>
+    <hyperlink ref="K12" r:id="rId9" xr:uid="{67D0D7A1-7FED-4116-87B2-323C2C487F80}"/>
+    <hyperlink ref="K13" r:id="rId10" xr:uid="{F214708D-00AD-4538-B55F-F8AE4F0DEBE8}"/>
+    <hyperlink ref="K14" r:id="rId11" xr:uid="{F518D799-3D99-4339-BAE6-5FA172B10A6E}"/>
+    <hyperlink ref="K15" r:id="rId12" xr:uid="{6797E9A2-B9EB-4895-94B1-429FC03897A3}"/>
+    <hyperlink ref="K6" r:id="rId13" xr:uid="{42EC9EA8-0236-4DA5-BA87-048F543CAA26}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes for Rev 1.1
</commit_message>
<xml_diff>
--- a/hw/ICEBoard Bill of Materials.xlsx
+++ b/hw/ICEBoard Bill of Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICEBoard\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE74228-BC56-4C01-9DC1-06A7E2617407}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD981D-7CA1-4D7A-9621-C146F4757701}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{71482D72-135C-40BB-96C7-234F6F45C228}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Type</t>
   </si>
@@ -84,21 +84,9 @@
     <t>D1, D2, D3, D4, D5, D6, D7, D8</t>
   </si>
   <si>
-    <t>DPDT</t>
-  </si>
-  <si>
     <t>C&amp;K</t>
   </si>
   <si>
-    <t>SWITCH SLIDE DPDT 300MA 6V</t>
-  </si>
-  <si>
-    <t>S1, S2, S3, S4</t>
-  </si>
-  <si>
-    <t>401-2002-1-ND</t>
-  </si>
-  <si>
     <t>Slide Switch</t>
   </si>
   <si>
@@ -213,9 +201,6 @@
     <t>PTS645SM50SMTR92 LFS</t>
   </si>
   <si>
-    <t>JS202011SCQN</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C4, C5, C6, C7, C8</t>
   </si>
   <si>
@@ -280,6 +265,36 @@
   </si>
   <si>
     <t>1276-6456-1-ND</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>SPDT</t>
+  </si>
+  <si>
+    <t>APEM</t>
+  </si>
+  <si>
+    <t>MHSS1104</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>S1, S2, S3, S4, S10</t>
+  </si>
+  <si>
+    <t>679-1848-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07470RL</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-470HRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -655,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57995C7-ECEF-42DD-8215-B17780662546}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -727,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I13" si="0">G2*H2</f>
+        <f t="shared" ref="I2:I14" si="0">G2*H2</f>
         <v>22</v>
       </c>
       <c r="J2" t="s">
@@ -742,7 +757,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -758,7 +773,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -790,55 +805,55 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="G5" s="1">
-        <v>0.48</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>1.92</v>
+        <v>2.75</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1">
         <v>0.26</v>
@@ -851,27 +866,27 @@
         <v>1.3</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1">
         <v>1.1200000000000001</v>
@@ -884,27 +899,27 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
       </c>
       <c r="G8" s="1">
         <v>1.95</v>
@@ -917,27 +932,27 @@
         <v>1.95</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>0.28000000000000003</v>
@@ -950,27 +965,27 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3">
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G10" s="5">
         <v>0.1</v>
@@ -983,27 +998,27 @@
         <v>0.4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G11" s="5">
         <v>0.1</v>
@@ -1016,106 +1031,139 @@
         <v>0.5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>470</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G12" s="5">
         <v>0.1</v>
       </c>
       <c r="H12" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G13" s="5">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="H13" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.8</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="G14" s="5">
-        <v>0.85</v>
+        <v>0.12</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" ref="I14" si="1">G14*H14</f>
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="5">
         <v>0.85</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>48</v>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" ref="I15" si="1">G15*H15</f>
+        <v>0.85</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished Rev 1.1 modifications
</commit_message>
<xml_diff>
--- a/hw/ICEBoard Bill of Materials.xlsx
+++ b/hw/ICEBoard Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICEBoard\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD981D-7CA1-4D7A-9621-C146F4757701}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C233BA1-259E-4B8A-A2D1-CB16DA4E2EE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{71482D72-135C-40BB-96C7-234F6F45C228}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Type</t>
   </si>
@@ -81,9 +81,6 @@
     <t>NeoPixel 5050 RGB LED with Integrated Driver Chip - 10 pack</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8</t>
-  </si>
-  <si>
     <t>C&amp;K</t>
   </si>
   <si>
@@ -153,12 +150,6 @@
     <t>PIEZO TRANSDUCER 5V 5mA 4kHz 75dB@5V, through hole</t>
   </si>
   <si>
-    <t>S5, S6, S7, S8, S9</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>2104-TP124005-2CT-ND</t>
   </si>
   <si>
@@ -295,6 +286,12 @@
   </si>
   <si>
     <t>311-470HRCT-ND</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8</t>
+  </si>
+  <si>
+    <t>BLeft, BUp, BCenter, BDown, BRight</t>
   </si>
 </sst>
 </file>
@@ -673,7 +670,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -757,7 +754,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -773,7 +770,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -787,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="G4" s="1">
         <v>4.5</v>
@@ -805,22 +802,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>85</v>
       </c>
       <c r="G5" s="1">
         <v>0.55000000000000004</v>
@@ -833,27 +830,27 @@
         <v>2.75</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="G6" s="1">
         <v>0.26</v>
@@ -866,27 +863,27 @@
         <v>1.3</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1">
         <v>1.1200000000000001</v>
@@ -899,27 +896,27 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>1.95</v>
@@ -932,27 +929,27 @@
         <v>1.95</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>0.28000000000000003</v>
@@ -965,27 +962,27 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3">
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G10" s="5">
         <v>0.1</v>
@@ -998,27 +995,27 @@
         <v>0.4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G11" s="5">
         <v>0.1</v>
@@ -1031,27 +1028,27 @@
         <v>0.5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>470</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G12" s="5">
         <v>0.1</v>
@@ -1064,27 +1061,27 @@
         <v>0.1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G13" s="5">
         <v>0.1</v>
@@ -1097,27 +1094,27 @@
         <v>0.8</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G14" s="5">
         <v>0.12</v>
@@ -1130,27 +1127,27 @@
         <v>0.12</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G15" s="5">
         <v>0.85</v>
@@ -1163,7 +1160,7 @@
         <v>0.85</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>